<commit_message>
check in basic problem from class and some LC
</commit_message>
<xml_diff>
--- a/Doc/狗家面经.xlsx
+++ b/Doc/狗家面经.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joanney1\Documents\Joanne's Data\mianjing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joanney1\Documents\Joanne's Data\LCProject\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,7 +747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>31</v>
@@ -925,15 +925,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A26:A28"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A21:A25"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A26:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>